<commit_message>
Updated Code for Excel and TestCaseSource
</commit_message>
<xml_diff>
--- a/EmployeeManagementAutomation/TestData/orange-test-data.xlsx
+++ b/EmployeeManagementAutomation/TestData/orange-test-data.xlsx
@@ -78,10 +78,10 @@
     <t>Time at Work</t>
   </si>
   <si>
-    <t>bala</t>
-  </si>
-  <si>
-    <t>bala1243</t>
+    <t>saul1</t>
+  </si>
+  <si>
+    <t>saul123</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added New TC AddEmployeeTest
</commit_message>
<xml_diff>
--- a/EmployeeManagementAutomation/TestData/orange-test-data.xlsx
+++ b/EmployeeManagementAutomation/TestData/orange-test-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="190" yWindow="490" windowWidth="18880" windowHeight="6740" activeTab="3"/>
+    <workbookView xWindow="190" yWindow="490" windowWidth="18880" windowHeight="6740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>firstname</t>
   </si>
   <si>
-    <t>middlename</t>
-  </si>
-  <si>
     <t>lastname</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>wick</t>
   </si>
   <si>
-    <t>jack2</t>
-  </si>
-  <si>
     <t>j2</t>
   </si>
   <si>
@@ -82,6 +76,12 @@
   </si>
   <si>
     <t>saul123</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>john</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -404,10 +404,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -436,7 +436,9 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -451,44 +453,44 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -515,18 +517,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>